<commit_message>
se ajusta informe planing
</commit_message>
<xml_diff>
--- a/Stefanini/Stefanini.Clientes/Stefanini.Cliente.Experian/Adopcion Safe.xlsx
+++ b/Stefanini/Stefanini.Clientes/Stefanini.Cliente.Experian/Adopcion Safe.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e10991a\Documents\Experian.Agile\Experian.Equipos\Experian.Nucleo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\omesan\Agile\Stefanini\Stefanini.Clientes\Stefanini.Cliente.Experian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F4E4EAE4-4412-4680-8955-68B2A34C9ECA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Adopcion Safe" sheetId="4" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>SGID</t>
   </si>
@@ -239,12 +238,15 @@
   </si>
   <si>
     <t>Logrado</t>
+  </si>
+  <si>
+    <t>Actual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -320,7 +322,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -515,6 +523,8 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,12 +577,423 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="es-CO" b="1"/>
+              <a:t>Marco</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CO" b="1" baseline="0"/>
+              <a:t> Safe</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CO" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$C$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Deseado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$B$47:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ceremonias</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Roles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$C$47:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F841-4247-BEA8-E4304AE0E292}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$D$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$B$47:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ceremonias</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Roles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$D$47:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41666666666666669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38412698412698409</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F841-4247-BEA8-E4304AE0E292}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1401665984"/>
+        <c:axId val="1401665568"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="1401665984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1401665568"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1401665568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1401665984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="es-CO"/>
               <a:t>Madurez Equipo</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -694,43 +1115,43 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.51724137931034486</c:v>
+                  <c:v>0.5357142857142857</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55172413793103448</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34482758620689657</c:v>
+                  <c:v>0.35714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55172413793103448</c:v>
+                  <c:v>0.5357142857142857</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17241379310344829</c:v>
+                  <c:v>0.17857142857142858</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2413793103448276</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31034482758620691</c:v>
+                  <c:v>0.32142857142857145</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44827586206896552</c:v>
+                  <c:v>0.4642857142857143</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.20689655172413793</c:v>
+                  <c:v>0.21428571428571427</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.27586206896551724</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.34482758620689657</c:v>
+                  <c:v>0.35714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.48275862068965519</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.31034482758620691</c:v>
+                  <c:v>0.32142857142857145</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1153,6 +1574,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1184,6 +1606,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1191,7 +1614,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1226,7 +1648,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -1274,6 +1696,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1365,7 +1788,7 @@
                   <c:v>0.29444444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31724137931034485</c:v>
+                  <c:v>0.32619047619047614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1638,6 +2061,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1669,6 +2093,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1676,7 +2101,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1752,6 +2176,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
@@ -2798,7 +3262,547 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190506</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238131</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3219,17 +4223,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A2:R43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G41" sqref="G41"/>
+      <selection pane="topRight" activeCell="D47" sqref="D47:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -4287,9 +5291,7 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2">
-        <v>1</v>
-      </c>
+      <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -4327,9 +5329,9 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="15"/>
@@ -4351,7 +5353,7 @@
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>SUM(A31:A37)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" s="23"/>
       <c r="C38" s="21"/>
@@ -4378,63 +5380,63 @@
         <v>16</v>
       </c>
       <c r="C39" s="24">
-        <f>SUM(C5:C14)/10</f>
+        <f>SUM(C5:C14)/$A$15</f>
         <v>0.4</v>
       </c>
       <c r="D39" s="24">
-        <f t="shared" ref="D39:Q39" si="0">SUM(D5:D14)/10</f>
+        <f>SUM(D5:D14)/$A$15</f>
         <v>0.4</v>
       </c>
       <c r="E39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(E5:E14)/$A$15</f>
         <v>0.2</v>
       </c>
       <c r="F39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(F5:F14)/$A$15</f>
         <v>0.4</v>
       </c>
       <c r="G39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(G5:G14)/$A$15</f>
         <v>0.1</v>
       </c>
       <c r="H39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(H5:H14)/$A$15</f>
         <v>0.3</v>
       </c>
       <c r="I39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(I5:I14)/$A$15</f>
         <v>0.2</v>
       </c>
       <c r="J39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(J5:J14)/$A$15</f>
         <v>0.3</v>
       </c>
       <c r="K39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(K5:K14)/$A$15</f>
         <v>0.1</v>
       </c>
       <c r="L39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(L5:L14)/$A$15</f>
         <v>0.1</v>
       </c>
       <c r="M39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(M5:M14)/$A$15</f>
         <v>0.2</v>
       </c>
       <c r="N39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(N5:N14)/$A$15</f>
         <v>0.6</v>
       </c>
       <c r="O39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(O5:O14)/$A$15</f>
         <v>0.4</v>
       </c>
       <c r="P39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(P5:P14)/$A$15</f>
         <v>0</v>
       </c>
       <c r="Q39" s="24">
-        <f t="shared" si="0"/>
+        <f>SUM(Q5:Q14)/$A$15</f>
         <v>0</v>
       </c>
       <c r="R39" s="16">
@@ -4447,67 +5449,67 @@
         <v>32</v>
       </c>
       <c r="C40" s="26">
-        <f>SUM(C17:C28)/12</f>
+        <f>SUM(C17:C28)/$A$29</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="D40" s="26">
-        <f t="shared" ref="D40:Q40" si="1">SUM(D17:D28)/12</f>
+        <f>SUM(D17:D28)/$A$29</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="E40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(E17:E28)/$A$29</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="F40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(F17:F28)/$A$29</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="G40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(G17:G28)/$A$29</f>
         <v>0</v>
       </c>
       <c r="H40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(H17:H28)/$A$29</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="I40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(I17:I28)/$A$29</f>
         <v>0.25</v>
       </c>
       <c r="J40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(J17:J28)/$A$29</f>
         <v>0.5</v>
       </c>
       <c r="K40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(K17:K28)/$A$29</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="L40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(L17:L28)/$A$29</f>
         <v>0.25</v>
       </c>
       <c r="M40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(M17:M28)/$A$29</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="N40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(N17:N28)/$A$29</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="O40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(O17:O28)/$A$29</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="P40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(P17:P28)/$A$29</f>
         <v>0</v>
       </c>
       <c r="Q40" s="26">
-        <f t="shared" si="1"/>
+        <f>SUM(Q17:Q28)/$A$29</f>
         <v>0</v>
       </c>
       <c r="R40" s="16">
-        <f t="shared" ref="R40:R42" si="2">AVERAGE(C40:Q40)</f>
+        <f t="shared" ref="R40:R42" si="0">AVERAGE(C40:Q40)</f>
         <v>0.29444444444444445</v>
       </c>
     </row>
@@ -4516,68 +5518,68 @@
         <v>55</v>
       </c>
       <c r="C41" s="26">
-        <f>SUM(C31:C37)/7</f>
-        <v>0.5714285714285714</v>
+        <f>SUM(C31:C37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D41" s="26">
-        <f t="shared" ref="D41:Q41" si="3">SUM(D31:D37)/7</f>
-        <v>0.5714285714285714</v>
+        <f>SUM(D31:D37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
+        <f>SUM(E31:E37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.7142857142857143</v>
+        <f>SUM(F31:F37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
+        <f>SUM(G31:G37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.42857142857142855</v>
+        <f>SUM(H31:H37)/$A$38</f>
+        <v>0.5</v>
       </c>
       <c r="I41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
+        <f>SUM(I31:I37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
+        <f>SUM(J31:J37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
+        <f>SUM(K31:K37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="L41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
+        <f>SUM(L31:L37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
+        <f>SUM(M31:M37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N41" s="26">
-        <f t="shared" si="3"/>
+        <f>SUM(N31:N37)/$A$38</f>
         <v>0</v>
       </c>
       <c r="O41" s="26">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
+        <f>SUM(O31:O37)/$A$38</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="P41" s="26">
-        <f t="shared" si="3"/>
+        <f>SUM(P31:P37)/$A$38</f>
         <v>0</v>
       </c>
       <c r="Q41" s="26">
-        <f t="shared" si="3"/>
+        <f>SUM(Q31:Q37)/$A$38</f>
         <v>0</v>
       </c>
       <c r="R41" s="16">
-        <f t="shared" si="2"/>
-        <v>0.45714285714285707</v>
+        <f t="shared" si="0"/>
+        <v>0.52222222222222237</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -4585,85 +5587,130 @@
         <v>67</v>
       </c>
       <c r="C42" s="25">
-        <f>SUM(C4:C37)/29</f>
-        <v>0.51724137931034486</v>
+        <f>SUM(C4:C37)/($A$38+$A$29+$A$15)</f>
+        <v>0.5357142857142857</v>
       </c>
       <c r="D42" s="25">
-        <f t="shared" ref="D42:Q42" si="4">SUM(D4:D37)/29</f>
-        <v>0.55172413793103448</v>
+        <f t="shared" ref="D42:Q42" si="1">SUM(D4:D37)/($A$38+$A$29+$A$15)</f>
+        <v>0.5714285714285714</v>
       </c>
       <c r="E42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.34482758620689657</v>
+        <f t="shared" si="1"/>
+        <v>0.35714285714285715</v>
       </c>
       <c r="F42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.55172413793103448</v>
+        <f t="shared" si="1"/>
+        <v>0.5357142857142857</v>
       </c>
       <c r="G42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.17241379310344829</v>
+        <f t="shared" si="1"/>
+        <v>0.17857142857142858</v>
       </c>
       <c r="H42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.2413793103448276</v>
+        <f t="shared" si="1"/>
+        <v>0.25</v>
       </c>
       <c r="I42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.31034482758620691</v>
+        <f t="shared" si="1"/>
+        <v>0.32142857142857145</v>
       </c>
       <c r="J42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.44827586206896552</v>
+        <f t="shared" si="1"/>
+        <v>0.4642857142857143</v>
       </c>
       <c r="K42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.20689655172413793</v>
+        <f t="shared" si="1"/>
+        <v>0.21428571428571427</v>
       </c>
       <c r="L42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.27586206896551724</v>
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
       </c>
       <c r="M42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.34482758620689657</v>
+        <f t="shared" si="1"/>
+        <v>0.35714285714285715</v>
       </c>
       <c r="N42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.48275862068965519</v>
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="O42" s="25">
-        <f t="shared" si="4"/>
-        <v>0.31034482758620691</v>
+        <f t="shared" si="1"/>
+        <v>0.32142857142857145</v>
       </c>
       <c r="P42" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q42" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R42" s="16">
-        <f t="shared" si="2"/>
-        <v>0.31724137931034485</v>
+        <f t="shared" si="0"/>
+        <v>0.32619047619047614</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C43" s="16"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="36">
+        <v>1</v>
+      </c>
+      <c r="D47" s="24">
+        <f>SUM(D13:D22)/$A$15</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="36">
+        <v>1</v>
+      </c>
+      <c r="D48" s="26">
+        <f>SUM(D25:D36)/$A$29</f>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="36">
+        <v>1</v>
+      </c>
+      <c r="D49" s="26">
+        <f>SUM(D39:D45)/$A$38</f>
+        <v>0.38412698412698409</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EB772F-2246-43D6-8E65-D259A2D4FD15}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4692,7 +5739,7 @@
       </c>
       <c r="C2" s="17">
         <f>'Adopcion Safe'!C42</f>
-        <v>0.51724137931034486</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="D2" s="20">
         <v>1</v>
@@ -4708,7 +5755,7 @@
       </c>
       <c r="C3" s="17">
         <f>'Adopcion Safe'!D42</f>
-        <v>0.55172413793103448</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="D3" s="20">
         <v>1</v>
@@ -4724,7 +5771,7 @@
       </c>
       <c r="C4" s="17">
         <f>'Adopcion Safe'!E42</f>
-        <v>0.34482758620689657</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="D4" s="20">
         <v>1</v>
@@ -4740,7 +5787,7 @@
       </c>
       <c r="C5" s="17">
         <f>'Adopcion Safe'!F42</f>
-        <v>0.55172413793103448</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="D5" s="20">
         <v>1</v>
@@ -4756,7 +5803,7 @@
       </c>
       <c r="C6" s="17">
         <f>'Adopcion Safe'!G42</f>
-        <v>0.17241379310344829</v>
+        <v>0.17857142857142858</v>
       </c>
       <c r="D6" s="20">
         <v>1</v>
@@ -4772,7 +5819,7 @@
       </c>
       <c r="C7" s="17">
         <f>'Adopcion Safe'!H42</f>
-        <v>0.2413793103448276</v>
+        <v>0.25</v>
       </c>
       <c r="D7" s="20">
         <v>1</v>
@@ -4788,7 +5835,7 @@
       </c>
       <c r="C8" s="17">
         <f>'Adopcion Safe'!I42</f>
-        <v>0.31034482758620691</v>
+        <v>0.32142857142857145</v>
       </c>
       <c r="D8" s="20">
         <v>1</v>
@@ -4804,7 +5851,7 @@
       </c>
       <c r="C9" s="17">
         <f>'Adopcion Safe'!J42</f>
-        <v>0.44827586206896552</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="D9" s="20">
         <v>1</v>
@@ -4820,7 +5867,7 @@
       </c>
       <c r="C10" s="17">
         <f>'Adopcion Safe'!K42</f>
-        <v>0.20689655172413793</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="D10" s="20">
         <v>1</v>
@@ -4836,7 +5883,7 @@
       </c>
       <c r="C11" s="17">
         <f>'Adopcion Safe'!L42</f>
-        <v>0.27586206896551724</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="D11" s="20">
         <v>1</v>
@@ -4852,7 +5899,7 @@
       </c>
       <c r="C12" s="17">
         <f>'Adopcion Safe'!M42</f>
-        <v>0.34482758620689657</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="D12" s="20">
         <v>1</v>
@@ -4868,7 +5915,7 @@
       </c>
       <c r="C13" s="17">
         <f>'Adopcion Safe'!N42</f>
-        <v>0.48275862068965519</v>
+        <v>0.5</v>
       </c>
       <c r="D13" s="20">
         <v>1</v>
@@ -4884,7 +5931,7 @@
       </c>
       <c r="C14" s="17">
         <f>'Adopcion Safe'!O42</f>
-        <v>0.31034482758620691</v>
+        <v>0.32142857142857145</v>
       </c>
       <c r="D14" s="20">
         <v>1</v>
@@ -4932,7 +5979,7 @@
       </c>
       <c r="C17" s="17">
         <f>AVERAGE(C2:C16)</f>
-        <v>0.31724137931034485</v>
+        <v>0.32619047619047614</v>
       </c>
       <c r="E17" s="29"/>
     </row>
@@ -4984,7 +6031,7 @@
       </c>
       <c r="C23" s="17">
         <f>'Adopcion Safe'!R42</f>
-        <v>0.31724137931034485</v>
+        <v>0.32619047619047614</v>
       </c>
       <c r="D23" s="27">
         <v>1</v>

</xml_diff>

<commit_message>
se ajusta informe planeacion
</commit_message>
<xml_diff>
--- a/Stefanini/Stefanini.Clientes/Stefanini.Cliente.Experian/Adopcion Safe.xlsx
+++ b/Stefanini/Stefanini.Clientes/Stefanini.Cliente.Experian/Adopcion Safe.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Adopcion Safe" sheetId="4" r:id="rId1"/>
-    <sheet name="RadarMadurez" sheetId="12" r:id="rId2"/>
+    <sheet name="Gráfico1" sheetId="13" r:id="rId1"/>
+    <sheet name="Adopcion Safe" sheetId="4" r:id="rId2"/>
+    <sheet name="RadarMadurez" sheetId="12" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
@@ -558,6 +559,3535 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$B$2:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$B$5:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$C$2:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Data Al día</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$C$5:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.58333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.5357142857142857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$D$2:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Decisor</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$D$5:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$E$2:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Célula Datos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$E$5:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.35714285714285715</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$F$2:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Seguros</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$F$5:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.58333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.5357142857142857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$G$2:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Validador de Ingreso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$G$5:$G$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.17857142857142858</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$H$2:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Antifraude</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$H$5:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$I$2:$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ebyington</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$I$5:$I$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.32142857142857145</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$J$2:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>APP</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$J$5:$J$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.4642857142857143</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>No bancarizado</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$K$5:$K$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.21428571428571427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$L$2:$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Seguridad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$L$5:$L$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$M$2:$M$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SME</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$M$5:$M$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.35714285714285715</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$N$2:$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SGID</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$N$5:$N$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$O$2:$O$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bus</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$O$5:$O$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.32142857142857145</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$P$2:$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Infraestructura</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$P$5:$P$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$Q$2:$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reconocer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$Q$5:$Q$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Adopcion Safe'!$R$2:$R$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Adopcion SaFe</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reconocer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Artefactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$A$5:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adopcion Safe'!$R$5:$R$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0%">
+                  <c:v>0.24666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0%">
+                  <c:v>0.29444444444444445</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0%">
+                  <c:v>0.52222222222222237</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0%">
+                  <c:v>0.32619047619047614</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-0318-4347-9915-D25988032935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="107033119"/>
+        <c:axId val="107033951"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="107033119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="107033951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="107033951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="107033119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -953,7 +4483,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -1648,7 +5178,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -2216,6 +5746,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
@@ -2253,7 +5823,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2457,6 +6027,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -2757,7 +6830,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3262,7 +7335,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3767,7 +7840,45 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="71" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9296937" cy="6063803"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3802,7 +7913,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4226,9 +8337,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D47" sqref="D47:D49"/>
+      <selection pane="topRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5380,63 +9491,63 @@
         <v>16</v>
       </c>
       <c r="C39" s="24">
-        <f>SUM(C5:C14)/$A$15</f>
+        <f t="shared" ref="C39:Q39" si="0">SUM(C5:C14)/$A$15</f>
         <v>0.4</v>
       </c>
       <c r="D39" s="24">
-        <f>SUM(D5:D14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="E39" s="24">
-        <f>SUM(E5:E14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="F39" s="24">
-        <f>SUM(F5:F14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="G39" s="24">
-        <f>SUM(G5:G14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="H39" s="24">
-        <f>SUM(H5:H14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="I39" s="24">
-        <f>SUM(I5:I14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="J39" s="24">
-        <f>SUM(J5:J14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="K39" s="24">
-        <f>SUM(K5:K14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="L39" s="24">
-        <f>SUM(L5:L14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="M39" s="24">
-        <f>SUM(M5:M14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="N39" s="24">
-        <f>SUM(N5:N14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="O39" s="24">
-        <f>SUM(O5:O14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="P39" s="24">
-        <f>SUM(P5:P14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q39" s="24">
-        <f>SUM(Q5:Q14)/$A$15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R39" s="16">
@@ -5449,67 +9560,67 @@
         <v>32</v>
       </c>
       <c r="C40" s="26">
-        <f>SUM(C17:C28)/$A$29</f>
+        <f t="shared" ref="C40:Q40" si="1">SUM(C17:C28)/$A$29</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="D40" s="26">
-        <f>SUM(D17:D28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E40" s="26">
-        <f>SUM(E17:E28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="F40" s="26">
-        <f>SUM(F17:F28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0.58333333333333337</v>
       </c>
       <c r="G40" s="26">
-        <f>SUM(G17:G28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H40" s="26">
-        <f>SUM(H17:H28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="I40" s="26">
-        <f>SUM(I17:I28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="J40" s="26">
-        <f>SUM(J17:J28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="K40" s="26">
-        <f>SUM(K17:K28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="L40" s="26">
-        <f>SUM(L17:L28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="M40" s="26">
-        <f>SUM(M17:M28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="N40" s="26">
-        <f>SUM(N17:N28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="O40" s="26">
-        <f>SUM(O17:O28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="P40" s="26">
-        <f>SUM(P17:P28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q40" s="26">
-        <f>SUM(Q17:Q28)/$A$29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R40" s="16">
-        <f t="shared" ref="R40:R42" si="0">AVERAGE(C40:Q40)</f>
+        <f t="shared" ref="R40:R42" si="2">AVERAGE(C40:Q40)</f>
         <v>0.29444444444444445</v>
       </c>
     </row>
@@ -5518,67 +9629,67 @@
         <v>55</v>
       </c>
       <c r="C41" s="26">
-        <f>SUM(C31:C37)/$A$38</f>
+        <f t="shared" ref="C41:Q41" si="3">SUM(C31:C37)/$A$38</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D41" s="26">
-        <f>SUM(D31:D37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E41" s="26">
-        <f>SUM(E31:E37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="F41" s="26">
-        <f>SUM(F31:F37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="G41" s="26">
-        <f>SUM(G31:G37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="H41" s="26">
-        <f>SUM(H31:H37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="I41" s="26">
-        <f>SUM(I31:I37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J41" s="26">
-        <f>SUM(J31:J37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="K41" s="26">
-        <f>SUM(K31:K37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="L41" s="26">
-        <f>SUM(L31:L37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="M41" s="26">
-        <f>SUM(M31:M37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="N41" s="26">
-        <f>SUM(N31:N37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O41" s="26">
-        <f>SUM(O31:O37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="P41" s="26">
-        <f>SUM(P31:P37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q41" s="26">
-        <f>SUM(Q31:Q37)/$A$38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R41" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.52222222222222237</v>
       </c>
     </row>
@@ -5591,63 +9702,63 @@
         <v>0.5357142857142857</v>
       </c>
       <c r="D42" s="25">
-        <f t="shared" ref="D42:Q42" si="1">SUM(D4:D37)/($A$38+$A$29+$A$15)</f>
+        <f t="shared" ref="D42:Q42" si="4">SUM(D4:D37)/($A$38+$A$29+$A$15)</f>
         <v>0.5714285714285714</v>
       </c>
       <c r="E42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="F42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="G42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.17857142857142858</v>
       </c>
       <c r="H42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
       <c r="I42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.32142857142857145</v>
       </c>
       <c r="J42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.4642857142857143</v>
       </c>
       <c r="K42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="L42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="M42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="N42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="O42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.32142857142857145</v>
       </c>
       <c r="P42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q42" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R42" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.32619047619047614</v>
       </c>
     </row>
@@ -5710,7 +9821,7 @@
   <dimension ref="B1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>